<commit_message>
midplate + chicker bom
</commit_message>
<xml_diff>
--- a/Chicker/POWER_BOARD_BOM_BASIC_TESTBOARD_JLC.xlsx
+++ b/Chicker/POWER_BOARD_BOM_BASIC_TESTBOARD_JLC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\henry\Documents\Documents\University\GitHub\The Bots\Electrical\PowerBoard\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\henry\Documents\Documents\University\GitHub\The_Bots\Electrical\Chicker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8455869-022B-476B-BC92-B2B13729E227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF3A8C65-9CB8-4245-AF2F-938DB5DB4AAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5112" yWindow="17172" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="POWER_BOARD" sheetId="1" r:id="rId1"/>
@@ -1393,7 +1393,7 @@
   <dimension ref="A1:L53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>